<commit_message>
added new snippets and worked on contact sheet
</commit_message>
<xml_diff>
--- a/JobContactSheet.xlsx
+++ b/JobContactSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\philliplagoc.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B175710D-B63E-480B-9192-F8464F201047}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5FC1467-A55E-410E-8072-34B8ED3856FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>Company Name</t>
   </si>
@@ -103,13 +103,37 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>Veeva</t>
+  </si>
+  <si>
+    <t>Applied at DECAF when I gave them my resume</t>
+  </si>
+  <si>
+    <t>Roivant</t>
+  </si>
+  <si>
+    <t>https://ripplematch.com/job/roivant/a4c935f2/</t>
+  </si>
+  <si>
+    <t>Tech Roivant Analyst Program 2020</t>
+  </si>
+  <si>
+    <t>Questionnaire needed and only one application; learned about through RippleMatch</t>
+  </si>
+  <si>
+    <t>RippleMatch</t>
+  </si>
+  <si>
+    <t>Yes (Why am I interested in working here?)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,6 +188,13 @@
       <name val="Bahnschrift"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Bahnschrift"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -186,7 +217,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -209,6 +240,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -495,8 +529,8 @@
   <dimension ref="A1:K84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C5" sqref="C5"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.6" x14ac:dyDescent="0.4"/>
@@ -612,27 +646,51 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="B5" s="4"/>
+    <row r="5" spans="1:11" ht="31.8" x14ac:dyDescent="0.4">
+      <c r="A5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="10"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+      <c r="E5" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
+      <c r="H5" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
+      <c r="J5" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="76.8" x14ac:dyDescent="0.4">
+      <c r="A6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
+      <c r="J6" s="4" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B7" s="4"/>
@@ -1496,8 +1554,9 @@
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{96E930A7-F871-4973-A53A-E63EA3FEF607}"/>
     <hyperlink ref="B4" r:id="rId2" xr:uid="{DCBF7BC9-2D3A-41E3-9597-1A6E71370305}"/>
+    <hyperlink ref="B6" r:id="rId3" xr:uid="{85CCB314-A3DD-4404-8045-9AE5D9F00616}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>